<commit_message>
Updated helper. Slowly moving away from it.... Using firebase objects directly in activities. Login works
</commit_message>
<xml_diff>
--- a/Projekt/TaskBoard.xlsx
+++ b/Projekt/TaskBoard.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t xml:space="preserve">AUH A30 </t>
   </si>
@@ -56,9 +56,6 @@
     <t>First time use (login screen)</t>
   </si>
   <si>
-    <t>Dashboard</t>
-  </si>
-  <si>
     <t>Staff</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
     <t>Make Firebase functions</t>
   </si>
   <si>
-    <t>Define baby attributes (Model)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Staff </t>
   </si>
   <si>
@@ -89,10 +83,19 @@
     <t>Listview adaptor to staff dashboard</t>
   </si>
   <si>
-    <t>Start on infortion section</t>
-  </si>
-  <si>
     <t>Mat</t>
+  </si>
+  <si>
+    <t>Mik</t>
+  </si>
+  <si>
+    <t>Start on information section</t>
+  </si>
+  <si>
+    <t>Detailed view for babies</t>
+  </si>
+  <si>
+    <t>Dashboard (Detailed view)</t>
   </si>
 </sst>
 </file>
@@ -190,7 +193,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -199,6 +202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="God" xfId="1" builtinId="26"/>
@@ -482,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D140"/>
+  <dimension ref="A1:D139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,101 +540,109 @@
         <v>9</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
+      <c r="C8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
+      <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
+      <c r="C12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
+        <v>22</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
@@ -1382,12 +1394,6 @@
       <c r="C139" s="5"/>
       <c r="D139" s="5"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A140" s="5"/>
-      <c r="B140" s="5"/>
-      <c r="C140" s="5"/>
-      <c r="D140" s="5"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>